<commit_message>
Make HTTP Callout From Lightning Component And Show Data inside Salesforce
</commit_message>
<xml_diff>
--- a/me/6.Callouts-using-Apex.xlsx
+++ b/me/6.Callouts-using-Apex.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce-integration-with-external-systems\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89410DAA-4C32-4FF3-A928-F7B28F52C8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FD0AF9-9653-4A3C-B0BC-CF29AA82F84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Remote site settings" sheetId="1" r:id="rId1"/>
     <sheet name="Create an Apex class" sheetId="2" r:id="rId2"/>
     <sheet name="MakeHttpCalloutFromLightningCmp" sheetId="3" r:id="rId3"/>
+    <sheet name="CalloutShowDataInsideSalesforce" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="370">
   <si>
     <t>構成</t>
   </si>
@@ -999,6 +1000,163 @@
   </si>
   <si>
     <t>SampleComponentHelper.txt</t>
+  </si>
+  <si>
+    <t>Make HTTP Callout From Lightning Component And Show Data inside Salesforce</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    @AuraEnabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    public static Map&lt;String,Object&gt; getCalloutResponseContents(String url)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Http h=new Http();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        HttpRequest req=new HttpRequest();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        req.setEndpoint(url);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        req.setMethod('GET');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        HttpResponse res=h.send(req);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        System.debug('response--&gt;: '+res.getBody());</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Map&lt;String,Object&gt; resultsMap=  (Map&lt;String,Object&gt;)JSON.deserializeUntyped(res.getBody());</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        System.debug('resultsMap '+resultsMap);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return resultsMap;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t>salesforce-integration-with-external-systems\6.Callouts-using-Apex\2.Make-HTTP-Callout-from-Lightning-component\SampleComponentController.txt</t>
+  </si>
+  <si>
+    <t>({</t>
+  </si>
+  <si>
+    <t>helper.getResponse(component);</t>
+  </si>
+  <si>
+    <t>})</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>calloutCtrl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : function(component, event, helper) {</t>
+    </r>
+  </si>
+  <si>
+    <t>salesforce-integration-with-external-systems\6.Callouts-using-Apex\2.Make-HTTP-Callout-from-Lightning-component\SampleComponentHelper.txt</t>
+  </si>
+  <si>
+    <t>getResponse : function(component) {</t>
+  </si>
+  <si>
+    <t>console.log('I m inside the helper');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        var action=component.get("c.getCalloutResponseContents");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        action.setParams({</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "url":'http://data.fixer.io/api/latest?access_key=738c44d040238a6f33970d76d41de37f'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        });</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        action.setCallback(this,function(response){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            var state=response.getState();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            if(component.isValid &amp;&amp; state==="SUCCESS")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                console.log('response.getReturnValue()=&gt; '+JSON.stringify(response.getReturnValue()));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                component.set("v.response",response.getReturnValue());</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                var getAllRates=component.get("v.response")['rates'];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                console.log('getAllRates=&gt;  '+JSON.stringify(getAllRates));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                var CurrencyList=[];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                for(var key in getAllRates)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    CurrencyList.push(key+'='+getAllRates[key]); //INR=70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                component.set("v.ListOfCurrency",CurrencyList);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                console.log('CurrencyList=&gt; '+CurrencyList);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             $A.enqueueAction(action);              </t>
+  </si>
+  <si>
+    <t>},</t>
+  </si>
+  <si>
+    <t>Check browser</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1141,17 +1299,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2452,6 +2603,187 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>59702</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7CE5878-4F26-B50E-160F-7027D874F133}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="19897725"/>
+          <a:ext cx="11229975" cy="5688977"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>56146</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F59AF894-6B33-3C41-3D11-0E506D3BFCC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="27308175"/>
+          <a:ext cx="11306175" cy="3227971"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>67235</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>123266</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>358589</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>49960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC169FD3-2372-B8AD-635F-0852BB6312EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="672353" y="31365266"/>
+          <a:ext cx="11183471" cy="2022194"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>333</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5534380-E61D-8CE4-2611-CCBD263A9CA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="33642300"/>
+          <a:ext cx="13011150" cy="32766000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3050,8 +3382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2C8266-6748-44DC-B747-461F9850EDA7}">
   <dimension ref="A2:T397"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I31"/>
+    <sheetView topLeftCell="A172" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5906,8 +6238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7AF866-C655-48CE-BB05-A52BCCBB509A}">
   <dimension ref="A2:O212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134"/>
+    <sheetView topLeftCell="A226" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5918,368 +6250,203 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="17"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="19"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="19"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="14" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="19"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14" t="s">
+      <c r="B9" s="5"/>
+      <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="19"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14" t="s">
+      <c r="B10" s="5"/>
+      <c r="E10" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="19"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
+      <c r="B11" s="5"/>
+      <c r="E11" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="19"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
+      <c r="B12" s="5"/>
+      <c r="E12" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="19"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
+      <c r="B13" s="5"/>
+      <c r="E13" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="19"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14" t="s">
+      <c r="B14" s="5"/>
+      <c r="F14" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="19"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14" t="s">
+      <c r="B15" s="5"/>
+      <c r="F15" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="19"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14" t="s">
+      <c r="B16" s="5"/>
+      <c r="F16" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="19"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14" t="s">
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="F17" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="19"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="14" t="s">
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="19"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14" t="s">
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="D19" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="19"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14" t="s">
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="D20" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="19"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14" t="s">
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="D21" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="19"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14" t="s">
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="E22" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="19"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14" t="s">
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="E23" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="19"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14" t="s">
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="D24" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="19"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14" t="s">
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="E25" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="19"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14" t="s">
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="E26" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="19"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="14" t="s">
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="19"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14" t="s">
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="D28" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="19"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14" t="s">
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="E29" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="19"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14" t="s">
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="E30" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="19"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="14"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
       <c r="D31" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="19"/>
+      <c r="I31" s="6"/>
       <c r="J31" t="s">
         <v>49</v>
       </c>
@@ -6287,68 +6454,43 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
       <c r="E32" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="19"/>
+      <c r="I32" s="6"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
+      <c r="B33" s="5"/>
       <c r="E33" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="19"/>
+      <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
+      <c r="B34" s="5"/>
       <c r="E34" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="19"/>
+      <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
+      <c r="B35" s="5"/>
       <c r="E35" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="19"/>
+      <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="22"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="9"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -6382,296 +6524,108 @@
       <c r="B89" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="C89" s="23"/>
-      <c r="D89" s="23"/>
-      <c r="E89" s="23"/>
-      <c r="F89" s="23"/>
-      <c r="G89" s="23"/>
-      <c r="H89" s="23"/>
-      <c r="I89" s="23"/>
-      <c r="J89" s="23"/>
-      <c r="K89" s="23"/>
-      <c r="L89" s="23"/>
-      <c r="M89" s="23"/>
-      <c r="N89" s="23"/>
       <c r="O89" s="6"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="C90" s="23"/>
-      <c r="D90" s="23"/>
-      <c r="E90" s="23"/>
-      <c r="F90" s="23"/>
-      <c r="G90" s="23"/>
-      <c r="H90" s="23"/>
-      <c r="I90" s="23"/>
-      <c r="J90" s="23"/>
-      <c r="K90" s="23"/>
-      <c r="L90" s="23"/>
-      <c r="M90" s="23"/>
-      <c r="N90" s="23"/>
       <c r="O90" s="6"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B91" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="C91" s="23"/>
-      <c r="D91" s="23"/>
-      <c r="E91" s="23"/>
-      <c r="F91" s="23"/>
-      <c r="G91" s="23"/>
-      <c r="H91" s="23"/>
-      <c r="I91" s="23"/>
-      <c r="J91" s="23"/>
-      <c r="K91" s="23"/>
-      <c r="L91" s="23"/>
-      <c r="M91" s="23"/>
-      <c r="N91" s="23"/>
       <c r="O91" s="6"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="C92" s="23" t="s">
+      <c r="C92" t="s">
         <v>298</v>
       </c>
-      <c r="D92" s="23"/>
-      <c r="E92" s="23"/>
-      <c r="F92" s="23"/>
-      <c r="G92" s="23"/>
-      <c r="H92" s="23"/>
-      <c r="I92" s="23"/>
-      <c r="J92" s="23"/>
-      <c r="K92" s="23"/>
-      <c r="L92" s="23"/>
-      <c r="M92" s="23"/>
-      <c r="N92" s="23"/>
       <c r="O92" s="6"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B93" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="C93" s="23" t="s">
+      <c r="C93" t="s">
         <v>300</v>
       </c>
-      <c r="D93" s="23"/>
-      <c r="E93" s="23"/>
-      <c r="F93" s="23"/>
-      <c r="G93" s="23"/>
-      <c r="H93" s="23"/>
-      <c r="I93" s="23"/>
-      <c r="J93" s="23"/>
-      <c r="K93" s="23"/>
-      <c r="L93" s="23"/>
-      <c r="M93" s="23"/>
-      <c r="N93" s="23"/>
       <c r="O93" s="6"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B94" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="C94" s="23"/>
-      <c r="D94" s="23"/>
-      <c r="E94" s="23"/>
-      <c r="F94" s="23"/>
-      <c r="G94" s="23"/>
-      <c r="H94" s="23"/>
-      <c r="I94" s="23"/>
-      <c r="J94" s="23"/>
-      <c r="K94" s="23"/>
-      <c r="L94" s="23"/>
-      <c r="M94" s="23"/>
-      <c r="N94" s="23"/>
       <c r="O94" s="6"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B95" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="C95" s="23"/>
-      <c r="D95" s="23"/>
-      <c r="E95" s="23"/>
-      <c r="F95" s="23"/>
-      <c r="G95" s="23"/>
-      <c r="H95" s="23"/>
-      <c r="I95" s="23"/>
-      <c r="J95" s="23"/>
-      <c r="K95" s="23"/>
-      <c r="L95" s="23"/>
-      <c r="M95" s="23"/>
-      <c r="N95" s="23"/>
       <c r="O95" s="6"/>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B96" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="C96" s="23"/>
-      <c r="D96" s="23"/>
-      <c r="E96" s="23"/>
-      <c r="F96" s="23"/>
-      <c r="G96" s="23"/>
-      <c r="H96" s="23"/>
-      <c r="I96" s="23"/>
-      <c r="J96" s="23"/>
-      <c r="K96" s="23"/>
-      <c r="L96" s="23"/>
-      <c r="M96" s="23"/>
-      <c r="N96" s="23"/>
       <c r="O96" s="6"/>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="C97" s="23"/>
-      <c r="D97" s="23"/>
-      <c r="E97" s="23"/>
-      <c r="F97" s="23"/>
-      <c r="G97" s="23"/>
-      <c r="H97" s="23"/>
-      <c r="I97" s="23"/>
-      <c r="J97" s="23"/>
-      <c r="K97" s="23"/>
-      <c r="L97" s="23"/>
-      <c r="M97" s="23"/>
-      <c r="N97" s="23"/>
       <c r="O97" s="6"/>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="C98" s="23"/>
-      <c r="D98" s="23"/>
-      <c r="E98" s="23"/>
-      <c r="F98" s="23"/>
-      <c r="G98" s="23"/>
-      <c r="H98" s="23"/>
-      <c r="I98" s="23"/>
-      <c r="J98" s="23"/>
-      <c r="K98" s="23"/>
-      <c r="L98" s="23"/>
-      <c r="M98" s="23"/>
-      <c r="N98" s="23"/>
       <c r="O98" s="6"/>
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="C99" s="23"/>
-      <c r="D99" s="23"/>
-      <c r="E99" s="23"/>
-      <c r="F99" s="23"/>
-      <c r="G99" s="23"/>
-      <c r="H99" s="23"/>
-      <c r="I99" s="23"/>
-      <c r="J99" s="23"/>
-      <c r="K99" s="23"/>
-      <c r="L99" s="23"/>
-      <c r="M99" s="23"/>
-      <c r="N99" s="23"/>
       <c r="O99" s="6"/>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C100" s="23"/>
-      <c r="D100" s="23"/>
-      <c r="E100" s="23"/>
-      <c r="F100" s="23"/>
-      <c r="G100" s="23"/>
-      <c r="H100" s="23"/>
-      <c r="I100" s="23"/>
-      <c r="J100" s="23"/>
-      <c r="K100" s="23"/>
-      <c r="L100" s="23"/>
-      <c r="M100" s="23"/>
-      <c r="N100" s="23"/>
       <c r="O100" s="6"/>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="C101" s="23" t="s">
+      <c r="C101" t="s">
         <v>306</v>
       </c>
-      <c r="D101" s="23"/>
-      <c r="E101" s="23"/>
-      <c r="F101" s="23"/>
-      <c r="G101" s="23"/>
-      <c r="H101" s="23"/>
-      <c r="I101" s="23"/>
-      <c r="J101" s="23"/>
-      <c r="K101" s="23"/>
-      <c r="L101" s="23"/>
-      <c r="M101" s="23"/>
-      <c r="N101" s="23"/>
       <c r="O101" s="6"/>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="C102" s="23" t="s">
+      <c r="C102" t="s">
         <v>307</v>
       </c>
-      <c r="D102" s="23"/>
-      <c r="E102" s="23"/>
-      <c r="F102" s="23"/>
-      <c r="G102" s="23"/>
-      <c r="H102" s="23"/>
-      <c r="I102" s="23"/>
-      <c r="J102" s="23"/>
-      <c r="K102" s="23"/>
-      <c r="L102" s="23"/>
-      <c r="M102" s="23"/>
-      <c r="N102" s="23"/>
       <c r="O102" s="6"/>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="C103" s="23"/>
-      <c r="D103" s="23"/>
-      <c r="E103" s="23"/>
-      <c r="F103" s="23"/>
-      <c r="G103" s="23"/>
-      <c r="H103" s="23"/>
-      <c r="I103" s="23"/>
-      <c r="J103" s="23"/>
-      <c r="K103" s="23"/>
-      <c r="L103" s="23"/>
-      <c r="M103" s="23"/>
-      <c r="N103" s="23"/>
       <c r="O103" s="6"/>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="C104" s="23"/>
-      <c r="D104" s="23"/>
-      <c r="E104" s="23"/>
-      <c r="F104" s="23"/>
-      <c r="G104" s="23"/>
-      <c r="H104" s="23"/>
-      <c r="I104" s="23"/>
-      <c r="J104" s="23"/>
-      <c r="K104" s="23"/>
-      <c r="L104" s="23"/>
-      <c r="M104" s="23"/>
-      <c r="N104" s="23"/>
       <c r="O104" s="6"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
@@ -6721,9 +6675,6 @@
       <c r="B190" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="C190" s="23"/>
-      <c r="D190" s="23"/>
-      <c r="E190" s="23"/>
       <c r="F190" s="6"/>
     </row>
     <row r="191" spans="2:8" x14ac:dyDescent="0.25">
@@ -6738,6 +6689,1012 @@
     <row r="212" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
         <v>317</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6CCB49-5C29-4B49-8399-1E8AB5F55578}">
+  <dimension ref="A2:L149"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A340" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U59" sqref="U59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="E27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="E30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="E31" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I31" s="6"/>
+      <c r="J31" t="s">
+        <v>49</v>
+      </c>
+      <c r="K31" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="D32" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="E33" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="E34" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="E35" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="I35" s="6"/>
+      <c r="J35" t="s">
+        <v>49</v>
+      </c>
+      <c r="K35" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="E36" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="I36" s="6"/>
+      <c r="J36" t="s">
+        <v>49</v>
+      </c>
+      <c r="K36" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="6"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="6"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="6"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="6"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="6"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="6"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="6"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="6"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="6"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="6"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="6"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="6"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="6"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="6"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="6"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" s="5"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="6"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="9"/>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B62" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="4"/>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B63" s="5"/>
+      <c r="C63" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="6"/>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B64" s="5"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="6"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="6"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B66" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="6"/>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B67" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="6"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B68" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="14"/>
+      <c r="L68" s="6"/>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B69" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="6"/>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B70" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="6"/>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="14"/>
+      <c r="L71" s="6"/>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B72" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="14"/>
+      <c r="L72" s="6"/>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B73" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="6"/>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="14"/>
+      <c r="L74" s="6"/>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B75" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="6"/>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B76" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="14"/>
+      <c r="K76" s="14"/>
+      <c r="L76" s="6"/>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B77" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="14"/>
+      <c r="L77" s="6"/>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B78" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+      <c r="K78" s="14"/>
+      <c r="L78" s="6"/>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B79" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="6"/>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B80" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
+      <c r="L80" s="6"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B81" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
+      <c r="L81" s="6"/>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B82" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="14"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
+      <c r="L82" s="6"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+      <c r="K83" s="14"/>
+      <c r="L83" s="6"/>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="6"/>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="14"/>
+      <c r="L85" s="6"/>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+      <c r="K86" s="14"/>
+      <c r="L86" s="6"/>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B87" s="5"/>
+      <c r="C87" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="14"/>
+      <c r="L87" s="6"/>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B88" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="8"/>
+      <c r="J88" s="8"/>
+      <c r="K88" s="8"/>
+      <c r="L88" s="9"/>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B123" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+      <c r="H123" s="4"/>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B124" s="5"/>
+      <c r="C124" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
+      <c r="F124" s="14"/>
+      <c r="G124" s="14"/>
+      <c r="H124" s="6"/>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B125" s="5"/>
+      <c r="C125" s="14"/>
+      <c r="D125" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="E125" s="14"/>
+      <c r="F125" s="14"/>
+      <c r="G125" s="14"/>
+      <c r="H125" s="6"/>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B126" s="5"/>
+      <c r="C126" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D126" s="14"/>
+      <c r="E126" s="14"/>
+      <c r="F126" s="14"/>
+      <c r="G126" s="14"/>
+      <c r="H126" s="6"/>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B127" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C127" s="8"/>
+      <c r="D127" s="8"/>
+      <c r="E127" s="8"/>
+      <c r="F127" s="8"/>
+      <c r="G127" s="8"/>
+      <c r="H127" s="9"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>